<commit_message>
[add] Proteccion de rutas por permiso
Se agrego la proteccion de rutas conforme a los permisos asignados
</commit_message>
<xml_diff>
--- a/public/templateActivos.xlsx
+++ b/public/templateActivos.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t># Activo</t>
   </si>
@@ -48,20 +48,26 @@
     <t>Usuario asignado</t>
   </si>
   <si>
-    <t>Fecha de asignacion</t>
-  </si>
-  <si>
     <t>REPORTE DE ACTIVOS PARA TI</t>
   </si>
   <si>
     <t>Aplicaciones</t>
+  </si>
+  <si>
+    <t>Fecha asignacion</t>
+  </si>
+  <si>
+    <t>Observaciones</t>
+  </si>
+  <si>
+    <t>Fecha baja</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -91,6 +97,12 @@
     </font>
     <font>
       <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -225,32 +237,62 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Buena" xfId="1" builtinId="26"/>
@@ -306,56 +348,14 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="1025" name="AutoShape 1" descr="https://file+.vscode-resource.vscode-cdn.net/c%3A/xampp/htdocs/ResidenciasSaray/public/resources/img/logo-DN.png?version%3D1666125129608"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="7277100" y="571500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>1876425</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
@@ -680,16 +680,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
@@ -697,11 +697,13 @@
     <col min="7" max="7" width="21.85546875" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" customWidth="1"/>
-    <col min="10" max="10" width="44.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="42.42578125" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="44.7109375" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -713,8 +715,10 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -726,8 +730,10 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -739,36 +745,41 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -780,8 +791,10 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -793,8 +806,10 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -806,8 +821,10 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>0</v>
       </c>
@@ -826,82 +843,99 @@
       <c r="F9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="I9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
-      <c r="L12" s="14"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
+      <c r="L9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="18"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="11"/>
+    </row>
+    <row r="13" spans="1:14" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="28" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="8:8" x14ac:dyDescent="0.25">
-      <c r="H29" s="10"/>
+      <c r="H29" s="5"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="1">
-    <mergeCell ref="C4:I5"/>
+    <mergeCell ref="F4:I5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>